<commit_message>
worked, but latter columns are not set values.
</commit_message>
<xml_diff>
--- a/intermediateTables/PreCATFishesOrigin.xlsx
+++ b/intermediateTables/PreCATFishesOrigin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\FGame\中鱼\StatDemo\intermediateTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{957C13AE-08C8-45F7-A767-B15213EECD16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07845B5B-0B8C-4E2B-8A4A-79EBE71BC6DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="鱼种设计表" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="960" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="286">
   <si>
     <t>鱼种</t>
   </si>
@@ -980,6 +980,26 @@
   </si>
   <si>
     <t>3、4</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水下结构体]开放水域</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水下结构体]水草</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水下结构体]石头</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水下结构体]沉木</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>水下结构体]桥墩</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1602,11 +1622,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BP24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H17" sqref="H17"/>
+      <selection pane="bottomRight" activeCell="R26" sqref="R26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1692,19 +1712,19 @@
         <v>207</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>5</v>
+        <v>281</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>6</v>
+        <v>282</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>7</v>
+        <v>283</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>8</v>
+        <v>284</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>9</v>
+        <v>285</v>
       </c>
       <c r="AA1" s="12" t="s">
         <v>208</v>
@@ -5667,10 +5687,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{662D3F43-4BA3-41B8-992B-9DA5624B5380}">
-  <dimension ref="A1:Q36"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5680,7 +5700,7 @@
     <col min="4" max="4" width="15.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="25" t="s">
         <v>125</v>
       </c>
@@ -5699,26 +5719,8 @@
       <c r="F1" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="J1" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="K1" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="L1" s="21" t="s">
-        <v>128</v>
-      </c>
-      <c r="M1" s="21" t="s">
-        <v>129</v>
-      </c>
-      <c r="N1" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="27" t="s">
         <v>131</v>
       </c>
@@ -5737,34 +5739,8 @@
       <c r="F2" s="28">
         <v>3.11</v>
       </c>
-      <c r="I2" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="K2" s="22" t="s">
-        <v>132</v>
-      </c>
-      <c r="L2" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="M2" s="22">
-        <v>1.24E-2</v>
-      </c>
-      <c r="N2" s="22">
-        <v>3.11</v>
-      </c>
-      <c r="P2">
-        <f>M2-E2</f>
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <f>N2-F2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>133</v>
       </c>
@@ -5783,34 +5759,8 @@
       <c r="F3" s="28">
         <v>3.05</v>
       </c>
-      <c r="I3" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="K3" s="22" t="s">
-        <v>134</v>
-      </c>
-      <c r="L3" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="M3" s="22">
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="N3" s="22">
-        <v>3.05</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P36" si="0">M3-E3</f>
-        <v>0</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q36" si="1">N3-F3</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>135</v>
       </c>
@@ -5829,34 +5779,8 @@
       <c r="F4" s="28">
         <v>3.28</v>
       </c>
-      <c r="I4" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="K4" s="22" t="s">
-        <v>135</v>
-      </c>
-      <c r="L4" s="22" t="s">
-        <v>54</v>
-      </c>
-      <c r="M4" s="22">
-        <v>6.1000000000000004E-3</v>
-      </c>
-      <c r="N4" s="22">
-        <v>3.28</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>136</v>
       </c>
@@ -5875,34 +5799,8 @@
       <c r="F5" s="28">
         <v>3.24</v>
       </c>
-      <c r="I5" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>136</v>
-      </c>
-      <c r="K5" s="22" t="s">
-        <v>137</v>
-      </c>
-      <c r="L5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="M5" s="22">
-        <v>7.9000000000000008E-3</v>
-      </c>
-      <c r="N5" s="22">
-        <v>3.24</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>138</v>
       </c>
@@ -5921,34 +5819,8 @@
       <c r="F6" s="28">
         <v>3.11</v>
       </c>
-      <c r="I6" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>138</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>139</v>
-      </c>
-      <c r="L6" s="22" t="s">
-        <v>57</v>
-      </c>
-      <c r="M6" s="22">
-        <v>8.0999999999999996E-3</v>
-      </c>
-      <c r="N6" s="22">
-        <v>3.11</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>140</v>
       </c>
@@ -5967,34 +5839,8 @@
       <c r="F7" s="28">
         <v>3.29</v>
       </c>
-      <c r="I7" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="K7" s="22" t="s">
-        <v>140</v>
-      </c>
-      <c r="L7" s="22" t="s">
-        <v>52</v>
-      </c>
-      <c r="M7" s="22">
-        <v>5.5999999999999999E-3</v>
-      </c>
-      <c r="N7" s="22">
-        <v>3.29</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>141</v>
       </c>
@@ -6013,34 +5859,8 @@
       <c r="F8" s="28">
         <v>3.14</v>
       </c>
-      <c r="I8" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="K8" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="L8" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="M8" s="22">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="N8" s="22">
-        <v>3.14</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>143</v>
       </c>
@@ -6059,34 +5879,8 @@
       <c r="F9" s="28">
         <v>3.28</v>
       </c>
-      <c r="I9" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="K9" s="22" t="s">
-        <v>144</v>
-      </c>
-      <c r="L9" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="M9" s="22">
-        <v>7.7000000000000002E-3</v>
-      </c>
-      <c r="N9" s="22">
-        <v>3.28</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>145</v>
       </c>
@@ -6105,34 +5899,8 @@
       <c r="F10" s="28">
         <v>3.2</v>
       </c>
-      <c r="I10" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>145</v>
-      </c>
-      <c r="K10" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="L10" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="M10" s="22">
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="N10" s="22">
-        <v>3.2</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>148</v>
       </c>
@@ -6151,34 +5919,8 @@
       <c r="F11" s="28">
         <v>3.01</v>
       </c>
-      <c r="I11" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="K11" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="L11" s="22" t="s">
-        <v>150</v>
-      </c>
-      <c r="M11" s="22">
-        <v>1.01E-2</v>
-      </c>
-      <c r="N11" s="22">
-        <v>3.01</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>151</v>
       </c>
@@ -6197,34 +5939,8 @@
       <c r="F12" s="28">
         <v>3</v>
       </c>
-      <c r="I12" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="K12" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="L12" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="M12" s="22">
-        <v>1.23E-2</v>
-      </c>
-      <c r="N12" s="22">
-        <v>3</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>152</v>
       </c>
@@ -6243,34 +5959,8 @@
       <c r="F13" s="28">
         <v>3.12</v>
       </c>
-      <c r="I13" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="K13" s="22" t="s">
-        <v>153</v>
-      </c>
-      <c r="L13" s="22" t="s">
-        <v>154</v>
-      </c>
-      <c r="M13" s="22">
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="N13" s="22">
-        <v>3.12</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="27" t="s">
         <v>155</v>
       </c>
@@ -6289,34 +5979,8 @@
       <c r="F14" s="28">
         <v>3.23</v>
       </c>
-      <c r="I14" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>155</v>
-      </c>
-      <c r="K14" s="22" t="s">
-        <v>156</v>
-      </c>
-      <c r="L14" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="M14" s="22">
-        <v>5.4000000000000003E-3</v>
-      </c>
-      <c r="N14" s="22">
-        <v>3.23</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="27" t="s">
         <v>157</v>
       </c>
@@ -6335,34 +5999,8 @@
       <c r="F15" s="28">
         <v>3.22</v>
       </c>
-      <c r="I15" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>157</v>
-      </c>
-      <c r="K15" s="22" t="s">
-        <v>158</v>
-      </c>
-      <c r="L15" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="M15" s="22">
-        <v>6.0000000000000001E-3</v>
-      </c>
-      <c r="N15" s="22">
-        <v>3.22</v>
-      </c>
-      <c r="P15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="27" t="s">
         <v>160</v>
       </c>
@@ -6381,34 +6019,8 @@
       <c r="F16" s="28">
         <v>2.96</v>
       </c>
-      <c r="I16" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="K16" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="L16" s="22" t="s">
-        <v>162</v>
-      </c>
-      <c r="M16" s="22">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="N16" s="22">
-        <v>2.96</v>
-      </c>
-      <c r="P16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="27" t="s">
         <v>163</v>
       </c>
@@ -6427,34 +6039,8 @@
       <c r="F17" s="28">
         <v>3</v>
       </c>
-      <c r="I17" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="K17" s="22" t="s">
-        <v>164</v>
-      </c>
-      <c r="L17" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="M17" s="22">
-        <v>1.2500000000000001E-2</v>
-      </c>
-      <c r="N17" s="22">
-        <v>3</v>
-      </c>
-      <c r="P17">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q17">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="27" t="s">
         <v>165</v>
       </c>
@@ -6473,34 +6059,8 @@
       <c r="F18" s="28">
         <v>3.23</v>
       </c>
-      <c r="I18" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>165</v>
-      </c>
-      <c r="K18" s="22" t="s">
-        <v>166</v>
-      </c>
-      <c r="L18" s="22" t="s">
-        <v>59</v>
-      </c>
-      <c r="M18" s="22">
-        <v>5.1999999999999998E-3</v>
-      </c>
-      <c r="N18" s="22">
-        <v>3.23</v>
-      </c>
-      <c r="P18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="27" t="s">
         <v>167</v>
       </c>
@@ -6519,34 +6079,8 @@
       <c r="F19" s="28">
         <v>3.1</v>
       </c>
-      <c r="I19" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="K19" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="L19" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="M19" s="22">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="N19" s="22">
-        <v>3.1</v>
-      </c>
-      <c r="P19">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="27" t="s">
         <v>169</v>
       </c>
@@ -6565,34 +6099,8 @@
       <c r="F20" s="28">
         <v>2.94</v>
       </c>
-      <c r="I20" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="L20" s="22" t="s">
-        <v>42</v>
-      </c>
-      <c r="M20" s="22">
-        <v>1.35E-2</v>
-      </c>
-      <c r="N20" s="22">
-        <v>2.94</v>
-      </c>
-      <c r="P20">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="27" t="s">
         <v>171</v>
       </c>
@@ -6611,34 +6119,8 @@
       <c r="F21" s="28">
         <v>3</v>
       </c>
-      <c r="I21" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>171</v>
-      </c>
-      <c r="K21" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="L21" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="M21" s="22">
-        <v>1.2E-2</v>
-      </c>
-      <c r="N21" s="22">
-        <v>3</v>
-      </c>
-      <c r="P21">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="27" t="s">
         <v>173</v>
       </c>
@@ -6657,34 +6139,8 @@
       <c r="F22" s="28">
         <v>3.02</v>
       </c>
-      <c r="I22" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>173</v>
-      </c>
-      <c r="K22" s="22" t="s">
-        <v>174</v>
-      </c>
-      <c r="L22" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="M22" s="22">
-        <v>1.18E-2</v>
-      </c>
-      <c r="N22" s="22">
-        <v>3.02</v>
-      </c>
-      <c r="P22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q22">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="27" t="s">
         <v>175</v>
       </c>
@@ -6703,34 +6159,8 @@
       <c r="F23" s="28">
         <v>3.27</v>
       </c>
-      <c r="I23" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>175</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="L23" s="22" t="s">
-        <v>177</v>
-      </c>
-      <c r="M23" s="22">
-        <v>5.7000000000000002E-3</v>
-      </c>
-      <c r="N23" s="22">
-        <v>3.27</v>
-      </c>
-      <c r="P23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q23">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="27" t="s">
         <v>178</v>
       </c>
@@ -6749,34 +6179,8 @@
       <c r="F24" s="28">
         <v>3.32</v>
       </c>
-      <c r="I24" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="L24" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="M24" s="22">
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="N24" s="22">
-        <v>3.32</v>
-      </c>
-      <c r="P24">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q24">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="27" t="s">
         <v>180</v>
       </c>
@@ -6795,34 +6199,8 @@
       <c r="F25" s="28">
         <v>3.27</v>
       </c>
-      <c r="I25" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="K25" s="22" t="s">
-        <v>180</v>
-      </c>
-      <c r="L25" s="22" t="s">
-        <v>50</v>
-      </c>
-      <c r="M25" s="22">
-        <v>5.1000000000000004E-3</v>
-      </c>
-      <c r="N25" s="22">
-        <v>3.27</v>
-      </c>
-      <c r="P25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="27" t="s">
         <v>181</v>
       </c>
@@ -6841,34 +6219,8 @@
       <c r="F26" s="28">
         <v>3</v>
       </c>
-      <c r="I26" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>181</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="L26" s="22" t="s">
-        <v>183</v>
-      </c>
-      <c r="M26" s="22">
-        <v>0.01</v>
-      </c>
-      <c r="N26" s="22">
-        <v>3</v>
-      </c>
-      <c r="P26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="27" t="s">
         <v>184</v>
       </c>
@@ -6887,34 +6239,8 @@
       <c r="F27" s="28">
         <v>3.02</v>
       </c>
-      <c r="I27" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>184</v>
-      </c>
-      <c r="K27" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="L27" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="M27" s="22">
-        <v>9.7999999999999997E-3</v>
-      </c>
-      <c r="N27" s="22">
-        <v>3.02</v>
-      </c>
-      <c r="P27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="27" t="s">
         <v>187</v>
       </c>
@@ -6933,34 +6259,8 @@
       <c r="F28" s="28">
         <v>3.16</v>
       </c>
-      <c r="I28" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="J28" s="22" t="s">
-        <v>187</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="L28" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="M28" s="22">
-        <v>1.0200000000000001E-2</v>
-      </c>
-      <c r="N28" s="22">
-        <v>3.16</v>
-      </c>
-      <c r="P28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q28">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="27" t="s">
         <v>189</v>
       </c>
@@ -6979,34 +6279,8 @@
       <c r="F29" s="28">
         <v>3.49</v>
       </c>
-      <c r="I29" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="J29" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="K29" s="22" t="s">
-        <v>190</v>
-      </c>
-      <c r="L29" s="22" t="s">
-        <v>191</v>
-      </c>
-      <c r="M29" s="22">
-        <v>8.9999999999999998E-4</v>
-      </c>
-      <c r="N29" s="22">
-        <v>3.49</v>
-      </c>
-      <c r="P29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q29">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="27" t="s">
         <v>192</v>
       </c>
@@ -7025,34 +6299,8 @@
       <c r="F30" s="28">
         <v>3.11</v>
       </c>
-      <c r="I30" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="K30" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="L30" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="M30" s="22">
-        <v>1.2800000000000001E-2</v>
-      </c>
-      <c r="N30" s="22">
-        <v>3.11</v>
-      </c>
-      <c r="P30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="27" t="s">
         <v>194</v>
       </c>
@@ -7071,34 +6319,8 @@
       <c r="F31" s="28">
         <v>3.09</v>
       </c>
-      <c r="I31" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>194</v>
-      </c>
-      <c r="K31" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="L31" s="22" t="s">
-        <v>69</v>
-      </c>
-      <c r="M31" s="22">
-        <v>1.32E-2</v>
-      </c>
-      <c r="N31" s="22">
-        <v>3.09</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="27" t="s">
         <v>196</v>
       </c>
@@ -7117,39 +6339,13 @@
       <c r="F32" s="40">
         <v>3.2</v>
       </c>
-      <c r="I32" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="J32" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="K32" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="L32" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="M32" s="22">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="N32" s="22">
-        <v>3.2</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="14" t="s">
         <v>151</v>
       </c>
       <c r="B33" t="str">
-        <f t="shared" ref="B33" si="2">SUBSTITUTE(C33," ","_")</f>
+        <f t="shared" ref="B33" si="0">SUBSTITUTE(C33," ","_")</f>
         <v>Tench</v>
       </c>
       <c r="C33" s="14" t="s">
@@ -7164,34 +6360,8 @@
       <c r="F33" s="14">
         <v>3</v>
       </c>
-      <c r="I33" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="J33" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="K33" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="L33" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="M33" s="22">
-        <v>1.23E-2</v>
-      </c>
-      <c r="N33" s="22">
-        <v>3</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="33" t="s">
         <v>167</v>
       </c>
@@ -7211,39 +6381,13 @@
       <c r="F34" s="14">
         <v>3.1</v>
       </c>
-      <c r="I34" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="K34" s="22" t="s">
-        <v>168</v>
-      </c>
-      <c r="L34" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="M34" s="22">
-        <v>9.5999999999999992E-3</v>
-      </c>
-      <c r="N34" s="22">
-        <v>3.1</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:17" ht="28.5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="34" t="s">
         <v>160</v>
       </c>
       <c r="B35" t="str">
-        <f t="shared" ref="B35:B36" si="3">SUBSTITUTE(C35," ","_")</f>
+        <f t="shared" ref="B35:B36" si="1">SUBSTITUTE(C35," ","_")</f>
         <v>White_Crappie</v>
       </c>
       <c r="C35" s="34" t="s">
@@ -7258,39 +6402,13 @@
       <c r="F35" s="14">
         <v>2.96</v>
       </c>
-      <c r="I35" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>160</v>
-      </c>
-      <c r="K35" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="L35" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="M35" s="22">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="N35" s="22">
-        <v>2.96</v>
-      </c>
-      <c r="P35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q35">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:17" ht="42.75" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>206</v>
       </c>
       <c r="B36" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="1"/>
         <v>White_Channel_Catfish</v>
       </c>
       <c r="C36" s="35" t="s">
@@ -7304,32 +6422,6 @@
       </c>
       <c r="F36" s="22">
         <v>3.11</v>
-      </c>
-      <c r="I36" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="J36" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="K36" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="L36" s="22" t="s">
-        <v>45</v>
-      </c>
-      <c r="M36" s="22">
-        <v>8.0999999999999996E-3</v>
-      </c>
-      <c r="N36" s="22">
-        <v>3.11</v>
-      </c>
-      <c r="P36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q36">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix issues that allocated prob weight is wrong
</commit_message>
<xml_diff>
--- a/intermediateTables/PreCATFishesOrigin.xlsx
+++ b/intermediateTables/PreCATFishesOrigin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DocsHDD\FGame\中鱼\StatDemo\intermediateTables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F682BFB-5682-49FF-80E9-8F197CAF89DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4319F71A-6D82-4D7A-91BE-FECB18A02B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="41685" windowHeight="18390" tabRatio="816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4290" yWindow="2490" windowWidth="41685" windowHeight="18390" tabRatio="816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="鱼种设计表" sheetId="1" r:id="rId1"/>
@@ -2179,7 +2179,7 @@
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D12" sqref="D12"/>
+      <selection pane="bottomRight" activeCell="A24" sqref="A24:XFD45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>